<commit_message>
add exit ? interrupt
</commit_message>
<xml_diff>
--- a/files/weather.xlsx
+++ b/files/weather.xlsx
@@ -488,32 +488,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Тверь</t>
+          <t>Сочи</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-11-25</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>З</t>
+          <t>В</t>
         </is>
       </c>
       <c r="F2" t="n">
         <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>990</v>
+        <v>1016</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -524,38 +524,38 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>2166</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Тверь</t>
+          <t>Сочи</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-11-25</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>З</t>
+          <t>В</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>990</v>
+        <v>1016</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -566,27 +566,27 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>2165</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Москва</t>
+          <t>Сочи</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-11-25</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -597,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>989</v>
+        <v>1016</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -608,38 +608,38 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>2164</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Пенза</t>
+          <t>Сочи</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-11-25</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ЮЗ</t>
+          <t>В</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>993</v>
+        <v>1016</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -650,13 +650,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>2163</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Пенза</t>
+          <t>Владивосток</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -666,22 +666,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="D6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
         <v>1</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ЮЗ</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>3</v>
-      </c>
       <c r="G6" t="n">
-        <v>993</v>
+        <v>1011</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -692,13 +692,13 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>2162</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Пенза</t>
+          <t>Владивосток</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -708,22 +708,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="D7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
         <v>1</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ЮЗ</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>3</v>
-      </c>
       <c r="G7" t="n">
-        <v>993</v>
+        <v>1011</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -734,13 +734,13 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>2161</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Москва</t>
+          <t>Владивосток</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -750,22 +750,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>С</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>З</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>2</v>
-      </c>
       <c r="G8" t="n">
-        <v>989</v>
+        <v>1011</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>2160</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="9">
@@ -792,7 +792,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -807,7 +807,7 @@
         <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>2159</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="10">
@@ -834,7 +834,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -849,7 +849,7 @@
         <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>2158</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="11">
@@ -876,7 +876,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14:15</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -888,10 +888,10 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>2157</v>
+        <v>2169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>